<commit_message>
Ya funciona el modelo de las 2 tabalas de estadísitcas, una general y una porpartido. En proceso la etapa de analsis
</commit_message>
<xml_diff>
--- a/1 - No code/docs/Analisys_match_nba.xlsx
+++ b/1 - No code/docs/Analisys_match_nba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\PycharmProjects\nba\1 - No code\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA6B34E-AABA-4074-9461-C7058C28EDD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EFE245-B674-40CF-92D3-AD8903EEA5EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{551C4716-7C71-4BA4-91AC-0CDE482C7BD1}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Nymburk - Opava" sheetId="3" r:id="rId1"/>
     <sheet name="Hoja1 (2)" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja2" sheetId="4" r:id="rId3"/>
+    <sheet name="Hoja2 (2)" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="42">
   <si>
     <t>q1</t>
   </si>
@@ -103,41 +104,74 @@
     <t>De visitante</t>
   </si>
   <si>
-    <t>Marca más de _ _ puntos en el Q_1</t>
-  </si>
-  <si>
-    <t>Marca más de _ _ puntos en el Q_2</t>
-  </si>
-  <si>
-    <t>Marca más de _ _ puntos en el Q_3</t>
-  </si>
-  <si>
-    <t>Su media esta:</t>
-  </si>
-  <si>
-    <t>Abajo_AVG: (↓AVG)</t>
-  </si>
-  <si>
-    <t>igual_AVG: (→AVG)</t>
-  </si>
-  <si>
-    <t>Arriba_AVG:(↑AVG)</t>
-  </si>
-  <si>
-    <t>El equipo supera su media del Q_4</t>
-  </si>
-  <si>
     <t>Va perdiendo por _ _ puntos al finalizar el Q_3</t>
   </si>
   <si>
     <t>Va ganando por _ _ puntos al finalizar el Q_3</t>
+  </si>
+  <si>
+    <t>Alcanza o supera un avg_q_1 (home o away) de:</t>
+  </si>
+  <si>
+    <t>Alcanza o supera un avg_q_2 (home o away) de:</t>
+  </si>
+  <si>
+    <t>Alcanza o supera un avg_q_3 (home o away) de:</t>
+  </si>
+  <si>
+    <t>El equipo supera su media historica  del Q_4, cuando al minuto 5 del q_4 del partido actual:</t>
+  </si>
+  <si>
+    <t>Su media del 4to cuarto avg_q_4 del partido actual (home o away) esta:</t>
+  </si>
+  <si>
+    <t>Abajo_AVG: (↓avg_gral_[h or a])</t>
+  </si>
+  <si>
+    <t>Arriba_AVG:(↑avg_gral_[h or a])</t>
+  </si>
+  <si>
+    <t>Abajo_AVG: (↓avg_q4_[h or a])</t>
+  </si>
+  <si>
+    <t>Arriba_AVG:(↑avg_q4_[h or a])</t>
+  </si>
+  <si>
+    <t>Igual_AVG: (→avg_q4_[h or a])</t>
+  </si>
+  <si>
+    <t>Igual_AVG: (→avg_gral_[h or a])</t>
+  </si>
+  <si>
+    <t>Abajo_MDN: (↓mdn_gral_[h or a])</t>
+  </si>
+  <si>
+    <t>Igual_MDN: (→mdn_gral_[h or a])</t>
+  </si>
+  <si>
+    <t>Arriba_MDN:(↑mdn_gral_[h or a])</t>
+  </si>
+  <si>
+    <t>Su media total comprendida entre q_1 a q_3 del aprtido actual (home o away) esta:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Su mediana total comprendida entre q_1 a q_3 del aprtido actual (home o away) esta: </t>
+  </si>
+  <si>
+    <t>Su media total comprendida entre q_1 a q_3 de un partido específico (home o away) esta:</t>
+  </si>
+  <si>
+    <t>Su media del 4to cuarto avg_q_4 de un partido específico (home o away) esta:</t>
+  </si>
+  <si>
+    <t>Su mediana … esta:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,6 +228,12 @@
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1835,7 +1875,7 @@
   <dimension ref="B2:R46"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1881,13 +1921,13 @@
         <v>30</v>
       </c>
       <c r="N2" s="15">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="O2" s="15">
         <v>1</v>
       </c>
       <c r="P2" s="15">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
@@ -1914,7 +1954,7 @@
         <v>19.13</v>
       </c>
       <c r="N3" s="15">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O3" s="15">
         <v>2</v>
@@ -1957,7 +1997,7 @@
         <v>3</v>
       </c>
       <c r="P4" s="15">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
@@ -1991,13 +2031,13 @@
         <v>76</v>
       </c>
       <c r="N5" s="15">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O5" s="15">
         <v>4</v>
       </c>
       <c r="P5" s="15">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
@@ -2026,26 +2066,26 @@
       </c>
       <c r="J6" s="5"/>
       <c r="N6" s="15">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O6" s="15">
         <v>5</v>
       </c>
       <c r="P6" s="15">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="H7" s="13"/>
       <c r="J7" s="5"/>
       <c r="N7" s="15">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="O7" s="15">
         <v>6</v>
       </c>
       <c r="P7" s="15">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
@@ -2072,14 +2112,12 @@
       </c>
       <c r="J8" s="5"/>
       <c r="N8" s="15">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="O8" s="15">
         <v>7</v>
       </c>
-      <c r="P8" s="15">
-        <v>17</v>
-      </c>
+      <c r="P8" s="15"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
@@ -2108,14 +2146,12 @@
       <c r="L9" s="17"/>
       <c r="M9" s="16"/>
       <c r="N9" s="15">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="O9" s="15">
         <v>8</v>
       </c>
-      <c r="P9" s="15">
-        <v>18</v>
-      </c>
+      <c r="P9" s="15"/>
       <c r="Q9" s="18"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
@@ -2149,14 +2185,12 @@
       <c r="L10" s="17"/>
       <c r="M10" s="16"/>
       <c r="N10" s="15">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="O10" s="15">
         <v>9</v>
       </c>
-      <c r="P10" s="15">
-        <v>19</v>
-      </c>
+      <c r="P10" s="15"/>
       <c r="R10" s="19"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
@@ -2189,15 +2223,11 @@
         <f>D11+E11+F11+H11</f>
         <v>92</v>
       </c>
-      <c r="N11" s="15">
-        <v>23</v>
-      </c>
+      <c r="N11" s="15"/>
       <c r="O11" s="15">
         <v>10</v>
       </c>
-      <c r="P11" s="15">
-        <v>22</v>
-      </c>
+      <c r="P11" s="15"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C12" s="8" t="s">
@@ -2223,15 +2253,11 @@
         <f>H11/L2</f>
         <v>1.6</v>
       </c>
-      <c r="N12" s="15">
-        <v>23</v>
-      </c>
+      <c r="N12" s="15"/>
       <c r="O12" s="15">
         <v>11</v>
       </c>
-      <c r="P12" s="15">
-        <v>23</v>
-      </c>
+      <c r="P12" s="15"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="H13" s="13"/>
@@ -2239,15 +2265,11 @@
         <f>J5+J11</f>
         <v>168</v>
       </c>
-      <c r="N13" s="15">
-        <v>25</v>
-      </c>
+      <c r="N13" s="15"/>
       <c r="O13" s="15">
         <v>12</v>
       </c>
-      <c r="P13" s="15">
-        <v>23</v>
-      </c>
+      <c r="P13" s="15"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
@@ -2273,50 +2295,38 @@
         <f t="shared" ref="H14" si="0">H6+H12</f>
         <v>3.5</v>
       </c>
-      <c r="N14" s="15">
-        <v>28</v>
-      </c>
+      <c r="N14" s="15"/>
       <c r="O14" s="15">
         <v>13</v>
       </c>
-      <c r="P14" s="15">
-        <v>23</v>
-      </c>
+      <c r="P14" s="15"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="H15" s="13"/>
-      <c r="N15" s="15">
-        <v>28</v>
-      </c>
+      <c r="N15" s="15"/>
       <c r="O15" s="15">
         <v>14</v>
       </c>
-      <c r="P15" s="15">
-        <v>27</v>
-      </c>
+      <c r="P15" s="15"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="N16" s="15">
-        <v>29</v>
-      </c>
+      <c r="N16" s="15"/>
       <c r="O16" s="15">
         <v>15</v>
       </c>
-      <c r="P16" s="15">
-        <v>31</v>
-      </c>
+      <c r="P16" s="15"/>
     </row>
     <row r="17" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="G17" s="6">
-        <f>AVERAGE(N2:N16)</f>
-        <v>22.133333333333333</v>
+        <f>AVERAGE(N2:N10)</f>
+        <v>21.777777777777779</v>
       </c>
       <c r="H17" s="6">
-        <f>AVERAGE(P2:P16)</f>
-        <v>19.133333333333333</v>
+        <f>AVERAGE(P2:P7)</f>
+        <v>18.833333333333332</v>
       </c>
       <c r="N17" s="15"/>
       <c r="O17" s="15">
@@ -2329,12 +2339,12 @@
         <v>15</v>
       </c>
       <c r="G18" s="6">
-        <f>MEDIAN(N2:N16)</f>
-        <v>22</v>
+        <f>MEDIAN(N2:N10)</f>
+        <v>19</v>
       </c>
       <c r="H18" s="6">
-        <f>MEDIAN(P2:P16)</f>
-        <v>18</v>
+        <f>MEDIAN(P2:P7)</f>
+        <v>19</v>
       </c>
       <c r="N18" s="15"/>
       <c r="O18" s="15">
@@ -2348,11 +2358,11 @@
       </c>
       <c r="G19" s="6">
         <f>G17-N2</f>
-        <v>4.1333333333333329</v>
+        <v>8.7777777777777786</v>
       </c>
       <c r="H19" s="6">
         <f>H17-P2</f>
-        <v>9.1333333333333329</v>
+        <v>6.8333333333333321</v>
       </c>
       <c r="N19" s="15"/>
       <c r="O19" s="15">
@@ -2365,12 +2375,12 @@
         <v>16</v>
       </c>
       <c r="G20" s="6">
-        <f>N16-G17</f>
-        <v>6.8666666666666671</v>
+        <f>N10-G17</f>
+        <v>9.2222222222222214</v>
       </c>
       <c r="H20" s="6">
-        <f>P16-H17</f>
-        <v>11.866666666666667</v>
+        <f>P7-H17</f>
+        <v>10.166666666666668</v>
       </c>
       <c r="N20" s="15"/>
       <c r="O20" s="15">
@@ -2666,85 +2676,235 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD256CD-DBCA-466D-A137-64BCA21F8F29}">
-  <dimension ref="B3:I8"/>
+  <dimension ref="B3:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" style="25" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="26" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" style="26" customWidth="1"/>
     <col min="3" max="3" width="16.140625" style="25" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="25" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" style="26" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" style="25" customWidth="1"/>
-    <col min="7" max="7" width="21" style="25" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" style="26" customWidth="1"/>
-    <col min="9" max="9" width="25.7109375" style="25" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="25"/>
+    <col min="4" max="4" width="36.85546875" style="25" customWidth="1"/>
+    <col min="5" max="5" width="39.140625" style="25" customWidth="1"/>
+    <col min="6" max="6" width="37.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" style="26" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="25" customWidth="1"/>
+    <col min="9" max="9" width="21" style="25" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" style="26" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" style="25" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="25"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" s="30" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" s="30" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="29"/>
-      <c r="D3" s="31" t="s">
-        <v>24</v>
+      <c r="D3" s="32" t="s">
+        <v>39</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="F3" s="32" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="G3" s="32" t="s">
         <v>23</v>
       </c>
       <c r="H3" s="32" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="I3" s="32" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="J3" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B4" s="32" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" s="31" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="28"/>
-      <c r="E4" s="27"/>
+      <c r="E4" s="28"/>
       <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="28"/>
       <c r="I4" s="28"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="27"/>
+      <c r="K4" s="28"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C5" s="31" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="28"/>
-      <c r="E5" s="27"/>
+      <c r="E5" s="28"/>
       <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="28"/>
       <c r="I5" s="28"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="27"/>
+      <c r="K5" s="28"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D6" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D7" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D8" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9438E770-9047-4823-9684-2F1BC6535F1A}">
+  <dimension ref="B3:K8"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" style="25" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" style="26" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="36.85546875" style="25" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" style="25" customWidth="1"/>
+    <col min="6" max="6" width="37.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" style="26" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="25" customWidth="1"/>
+    <col min="9" max="9" width="21" style="25" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" style="26" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" style="25" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="25"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:11" s="30" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="29"/>
+      <c r="D3" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="32" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="B4" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="28"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C5" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="28"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D6" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D7" s="28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D8" s="28" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ya tengo identificados los punsto en la grafica según el rango de los promedios de Q_1 a Q_3. Ahora determinar como la media de los rangos se relaciona con las media de los datos y la línea de tendencia de regresión lineal
</commit_message>
<xml_diff>
--- a/1 - No code/docs/Analisys_match_nba.xlsx
+++ b/1 - No code/docs/Analisys_match_nba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\PycharmProjects\nba\1 - No code\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AC1E3F-85E2-4A3F-82E1-84B3F84CD770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52518BBA-8F74-4CF6-9556-C7F886A9B095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="772" activeTab="5" xr2:uid="{551C4716-7C71-4BA4-91AC-0CDE482C7BD1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="772" activeTab="6" xr2:uid="{551C4716-7C71-4BA4-91AC-0CDE482C7BD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Nymburk - Opava" sheetId="3" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="143">
   <si>
     <t>q1</t>
   </si>
@@ -486,6 +486,21 @@
   <si>
     <t>Corr 1-3</t>
   </si>
+  <si>
+    <t>Std</t>
+  </si>
+  <si>
+    <t>Range Total</t>
+  </si>
+  <si>
+    <t>Range Q1-Q2</t>
+  </si>
+  <si>
+    <t>Range Q1-Q3</t>
+  </si>
+  <si>
+    <t>Range Q2-Q3</t>
+  </si>
 </sst>
 </file>
 
@@ -705,7 +720,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -785,11 +800,70 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1152,11 +1226,72 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="48">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1296,6 +1431,364 @@
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -7372,8 +7865,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -7873,8 +8367,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -8368,8 +8863,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -26929,38 +27425,71 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{64A52F8A-FD08-448E-A26A-76A8C69B4176}" name="Tabla1" displayName="Tabla1" ref="D24:P44" totalsRowShown="0" headerRowDxfId="33" tableBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{64A52F8A-FD08-448E-A26A-76A8C69B4176}" name="Tabla1" displayName="Tabla1" ref="D24:P44" totalsRowShown="0" headerRowDxfId="47" tableBorderDxfId="46">
   <autoFilter ref="D24:P44" xr:uid="{64A52F8A-FD08-448E-A26A-76A8C69B4176}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D25:P44">
     <sortCondition ref="H24:H44"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{C498B744-819C-4C30-AD89-8D010C8DD57F}" name="Columna1" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{963426E7-A6EC-4E2B-8FA8-4C25DE6F27F1}" name="AVG_Q1_Q3" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{022AE098-8152-4412-B21F-798053AB0FEF}" name="Diff_Q3" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{C498B744-819C-4C30-AD89-8D010C8DD57F}" name="Columna1" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{963426E7-A6EC-4E2B-8FA8-4C25DE6F27F1}" name="AVG_Q1_Q3" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{022AE098-8152-4412-B21F-798053AB0FEF}" name="Diff_Q3" dataDxfId="43"/>
     <tableColumn id="4" xr3:uid="{6C751D08-5075-4887-8AC2-66C658B612F6}" name="Diff_Final"/>
-    <tableColumn id="5" xr3:uid="{61687A36-C0A6-4149-A42E-70B9983F7488}" name="AVG_MATCH" dataDxfId="28"/>
-    <tableColumn id="12" xr3:uid="{BC05FD90-7F89-41ED-AADC-4604DC568D8A}" name="Columna3" dataDxfId="27">
+    <tableColumn id="5" xr3:uid="{61687A36-C0A6-4149-A42E-70B9983F7488}" name="AVG_MATCH" dataDxfId="42"/>
+    <tableColumn id="12" xr3:uid="{BC05FD90-7F89-41ED-AADC-4604DC568D8A}" name="Columna3" dataDxfId="41">
       <calculatedColumnFormula>(Tabla1[[#This Row],[AVG_MATCH]]-$H$47)/$H$50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{49A84104-9446-489E-8C61-2ED6D92CC866}" name="Pronóstico" dataDxfId="26">
+    <tableColumn id="6" xr3:uid="{49A84104-9446-489E-8C61-2ED6D92CC866}" name="Pronóstico" dataDxfId="40">
       <calculatedColumnFormula xml:space="preserve"> $B$17+$B$18*E25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EE4C6112-9943-470C-A96A-053C93E3455B}" name="Pronostico - sdt_error" dataDxfId="25">
+    <tableColumn id="7" xr3:uid="{EE4C6112-9943-470C-A96A-053C93E3455B}" name="Pronostico - sdt_error" dataDxfId="39">
       <calculatedColumnFormula>J25-$B$7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{D66B6166-C397-49A9-996D-C2F46C07FF76}" name="Pronostico + sdt_error" dataDxfId="24">
+    <tableColumn id="8" xr3:uid="{D66B6166-C397-49A9-996D-C2F46C07FF76}" name="Pronostico + sdt_error" dataDxfId="38">
       <calculatedColumnFormula>J25+$B$7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{44A8EC7F-DA8F-483C-8272-4B6D26503747}" name="Diferencia entre el pronostico y avg_q1_q3" dataDxfId="23">
+    <tableColumn id="9" xr3:uid="{44A8EC7F-DA8F-483C-8272-4B6D26503747}" name="Diferencia entre el pronostico y avg_q1_q3" dataDxfId="37">
       <calculatedColumnFormula>J25-E25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5ACA37FE-8420-4221-B5C6-EE61DD3F44FC}" name="↑ Avg_match" dataDxfId="22">
+    <tableColumn id="10" xr3:uid="{5ACA37FE-8420-4221-B5C6-EE61DD3F44FC}" name="↑ Avg_match" dataDxfId="36">
       <calculatedColumnFormula>H25-E25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{F7F7B7FE-A536-4884-A0E7-B355357E46C1}" name="Is_Win" dataDxfId="21"/>
-    <tableColumn id="13" xr3:uid="{82641514-7132-414E-BFB3-1A8A2F1124A6}" name="Columna2" dataDxfId="20">
+    <tableColumn id="11" xr3:uid="{F7F7B7FE-A536-4884-A0E7-B355357E46C1}" name="Is_Win" dataDxfId="35"/>
+    <tableColumn id="13" xr3:uid="{82641514-7132-414E-BFB3-1A8A2F1124A6}" name="Columna2" dataDxfId="34">
       <calculatedColumnFormula>Tabla1[[#This Row],[AVG_MATCH]]-H24</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{485E2BCA-19BE-4688-813A-5AC9E231C9DE}" name="Tabla2" displayName="Tabla2" ref="W3:AE12" totalsRowShown="0" headerRowDxfId="25" dataDxfId="26" headerRowBorderDxfId="32" tableBorderDxfId="33" totalsRowBorderDxfId="31">
+  <autoFilter ref="W3:AE12" xr:uid="{485E2BCA-19BE-4688-813A-5AC9E231C9DE}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="W4:AB12">
+    <sortCondition ref="Z3:Z12"/>
+  </sortState>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{2671FE0E-309D-4528-9D6D-FFC95152AA55}" name="Q1" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{A506DEDE-3EE5-4B0E-9DAF-049F016C77A5}" name="Q2" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{E3E0F319-5B16-44A3-9BA9-0E50205F8CAC}" name="Q3" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{2871D33B-BA28-4DE8-8EE7-B1EE985FCCD0}" name="Range Total" dataDxfId="27">
+      <calculatedColumnFormula>MAX(W4:Y4)-MIN(W4:Y4)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{D8C93832-4F9A-4763-9AC9-1682B44C2048}" name="Range Q1-Q2" dataDxfId="22">
+      <calculatedColumnFormula>MAX(Tabla2[[#This Row],[Q1]:[Q2]])-MIN(Tabla2[[#This Row],[Q1]:[Q2]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{5C654CAC-82E2-4598-9FD4-CB25ECEBAD11}" name="Range Q1-Q3" dataDxfId="21">
+      <calculatedColumnFormula>MAX(W4,Y4)-MIN(W4,Y4)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{7386E846-9504-4E6B-875C-597C51781228}" name="Range Q2-Q3" dataDxfId="0">
+      <calculatedColumnFormula>MAX(X4,Y4)-MIN(X4,Y4)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{9F6E5363-5324-4E79-8808-747235B2F644}" name="Media" dataDxfId="24">
+      <calculatedColumnFormula>AVERAGE(W4:Y4)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{BD75AC7D-E54B-497D-B8F0-3744796B5162}" name="Std" dataDxfId="23">
+      <calculatedColumnFormula>_xlfn.STDEV.S(W4:Y4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -28042,82 +28571,82 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="19" priority="19">
+    <cfRule type="expression" dxfId="20" priority="19">
       <formula>$D$6&gt;$D$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="20">
+    <cfRule type="expression" dxfId="19" priority="20">
       <formula>$D$6&lt;$D$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="expression" dxfId="17" priority="17">
+    <cfRule type="expression" dxfId="18" priority="17">
       <formula>$E$6&gt;$E$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="18">
+    <cfRule type="expression" dxfId="17" priority="18">
       <formula>$E$6&lt;$E$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="expression" dxfId="15" priority="15">
+    <cfRule type="expression" dxfId="16" priority="15">
       <formula>$F$6&gt;$F$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="16">
+    <cfRule type="expression" dxfId="15" priority="16">
       <formula>$F$6&lt;$F$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="expression" dxfId="13" priority="13">
+    <cfRule type="expression" dxfId="14" priority="13">
       <formula>$G$6&gt;$G$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="14">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>$G$6&lt;$G$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="expression" dxfId="11" priority="11">
+    <cfRule type="expression" dxfId="12" priority="11">
       <formula>$D$12&gt;$D$10</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="11" priority="12">
       <formula>$D$12&lt;$D$10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="expression" dxfId="9" priority="9">
+    <cfRule type="expression" dxfId="10" priority="9">
       <formula>$E$12&gt;$E$10</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="10">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>$E$12&lt;$E$10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="8" priority="7">
       <formula>$F$12&gt;$F$10</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>$F$12&lt;$F$10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>$G$12&gt;$G$10</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>$G$12&lt;$G$10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>$H$6&gt;$H$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$H$6&lt;$H$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$H$12&gt;$H$10</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$H$12&lt;$H$10</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34270,8 +34799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A187434-1317-4278-823E-381B97E2F0CC}">
   <dimension ref="C1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34698,10 +35227,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC76F1D7-E302-4C94-B269-BE3976196AE2}">
-  <dimension ref="A2:M143"/>
+  <dimension ref="A2:AE143"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34711,10 +35240,16 @@
     <col min="4" max="7" width="11.42578125" style="54"/>
     <col min="8" max="8" width="16.85546875" style="54" customWidth="1"/>
     <col min="9" max="9" width="18.85546875" style="104" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="54"/>
+    <col min="10" max="21" width="11.42578125" style="54"/>
+    <col min="22" max="22" width="3.7109375" style="54" customWidth="1"/>
+    <col min="23" max="25" width="11.42578125" style="54"/>
+    <col min="26" max="26" width="14.7109375" style="54" customWidth="1"/>
+    <col min="27" max="27" width="18" style="54" customWidth="1"/>
+    <col min="28" max="29" width="21.28515625" style="54" customWidth="1"/>
+    <col min="30" max="16384" width="11.42578125" style="54"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="H2" s="53" t="s">
         <v>96</v>
       </c>
@@ -34722,7 +35257,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">
         <v>81</v>
       </c>
@@ -34751,8 +35286,35 @@
       <c r="L3" s="51">
         <v>0</v>
       </c>
+      <c r="W3" s="128" t="s">
+        <v>123</v>
+      </c>
+      <c r="X3" s="129" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y3" s="129" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z3" s="129" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA3" s="129" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB3" s="129" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC3" s="129" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD3" s="129" t="s">
+        <v>92</v>
+      </c>
+      <c r="AE3" s="129" t="s">
+        <v>138</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="56">
         <f>Avg_Match!E25</f>
         <v>1.5333330000000001</v>
@@ -34789,8 +35351,41 @@
         <f t="shared" ref="L4:L23" si="1">_xlfn.NORM.DIST(G4, $G$25,$G$28,1)</f>
         <v>5.4159690365002011E-2</v>
       </c>
+      <c r="W4" s="126">
+        <v>0.7</v>
+      </c>
+      <c r="X4" s="105">
+        <v>1.6</v>
+      </c>
+      <c r="Y4" s="105">
+        <v>1.7</v>
+      </c>
+      <c r="Z4" s="105">
+        <f>MAX(W4:Y4)-MIN(W4:Y4)</f>
+        <v>1</v>
+      </c>
+      <c r="AA4" s="105">
+        <f>MAX(Tabla2[[#This Row],[Q1]:[Q2]])-MIN(Tabla2[[#This Row],[Q1]:[Q2]])</f>
+        <v>0.90000000000000013</v>
+      </c>
+      <c r="AB4" s="105">
+        <f t="shared" ref="AB4:AB12" si="2">MAX(W4,Y4)-MIN(W4,Y4)</f>
+        <v>1</v>
+      </c>
+      <c r="AC4" s="134">
+        <f t="shared" ref="AC4:AC12" si="3">MAX(X4,Y4)-MIN(X4,Y4)</f>
+        <v>9.9999999999999867E-2</v>
+      </c>
+      <c r="AD4" s="134">
+        <f>AVERAGE(W4:Y4)</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="AE4" s="134">
+        <f>_xlfn.STDEV.S(W4:Y4)</f>
+        <v>0.55075705472861014</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="56">
         <f>Avg_Match!E26</f>
         <v>1.8666670000000001</v>
@@ -34812,11 +35407,11 @@
         <v>2</v>
       </c>
       <c r="H5" s="51">
-        <f t="shared" ref="H5:H22" si="2">_xlfn.NORM.DIST(G5,$G$25,$G$28, 1)</f>
+        <f t="shared" ref="H5:H22" si="4">_xlfn.NORM.DIST(G5,$G$25,$G$28, 1)</f>
         <v>7.5392782513985637E-2</v>
       </c>
       <c r="I5" s="121">
-        <f t="shared" ref="I5:I23" si="3">_xlfn.NORM.DIST(G5,$G$25,$G$28, 0)</f>
+        <f t="shared" ref="I5:I23" si="5">_xlfn.NORM.DIST(G5,$G$25,$G$28, 0)</f>
         <v>2.4022715404011696E-2</v>
       </c>
       <c r="K5" s="51">
@@ -34827,8 +35422,41 @@
         <f t="shared" si="1"/>
         <v>7.5392782513985637E-2</v>
       </c>
+      <c r="W5" s="126">
+        <v>1.5</v>
+      </c>
+      <c r="X5" s="105">
+        <v>2</v>
+      </c>
+      <c r="Y5" s="105">
+        <v>0.6</v>
+      </c>
+      <c r="Z5" s="105">
+        <f>MAX(W5:Y5)-MIN(W5:Y5)</f>
+        <v>1.4</v>
+      </c>
+      <c r="AA5" s="107">
+        <f>MAX(Tabla2[[#This Row],[Q1]:[Q2]])-MIN(Tabla2[[#This Row],[Q1]:[Q2]])</f>
+        <v>0.5</v>
+      </c>
+      <c r="AB5" s="127">
+        <f t="shared" si="2"/>
+        <v>0.9</v>
+      </c>
+      <c r="AC5" s="127">
+        <f t="shared" si="3"/>
+        <v>1.4</v>
+      </c>
+      <c r="AD5" s="105">
+        <f>AVERAGE(W5:Y5)</f>
+        <v>1.3666666666666665</v>
+      </c>
+      <c r="AE5" s="105">
+        <f>_xlfn.STDEV.S(W5:Y5)</f>
+        <v>0.70945988845975916</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="56">
         <f>Avg_Match!E27</f>
         <v>1.6333329999999999</v>
@@ -34850,11 +35478,11 @@
         <v>3</v>
       </c>
       <c r="H6" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.10244694690818926</v>
       </c>
       <c r="I6" s="121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.019182784072922E-2</v>
       </c>
       <c r="K6" s="51">
@@ -34865,8 +35493,41 @@
         <f t="shared" si="1"/>
         <v>0.10244694690818926</v>
       </c>
+      <c r="W6" s="126">
+        <v>2.1</v>
+      </c>
+      <c r="X6" s="105">
+        <v>2</v>
+      </c>
+      <c r="Y6" s="105">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Z6" s="105">
+        <f>MAX(W6:Y6)-MIN(W6:Y6)</f>
+        <v>0.29999999999999982</v>
+      </c>
+      <c r="AA6" s="107">
+        <f>MAX(Tabla2[[#This Row],[Q1]:[Q2]])-MIN(Tabla2[[#This Row],[Q1]:[Q2]])</f>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="AB6" s="127">
+        <f t="shared" si="2"/>
+        <v>0.19999999999999973</v>
+      </c>
+      <c r="AC6" s="127">
+        <f t="shared" si="3"/>
+        <v>0.29999999999999982</v>
+      </c>
+      <c r="AD6" s="105">
+        <f>AVERAGE(W6:Y6)</f>
+        <v>2.1333333333333333</v>
+      </c>
+      <c r="AE6" s="105">
+        <f>_xlfn.STDEV.S(W6:Y6)</f>
+        <v>0.15275252316519458</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="56">
         <f>Avg_Match!E28</f>
         <v>1.8333330000000001</v>
@@ -34888,11 +35549,11 @@
         <v>4</v>
       </c>
       <c r="H7" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.1359493554098242</v>
       </c>
       <c r="I7" s="121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.687638179856368E-2</v>
       </c>
       <c r="K7" s="51">
@@ -34903,8 +35564,41 @@
         <f t="shared" si="1"/>
         <v>0.1359493554098242</v>
       </c>
+      <c r="W7" s="126">
+        <v>1.4</v>
+      </c>
+      <c r="X7" s="105">
+        <v>1.6</v>
+      </c>
+      <c r="Y7" s="105">
+        <v>1.71</v>
+      </c>
+      <c r="Z7" s="105">
+        <f>MAX(W7:Y7)-MIN(W7:Y7)</f>
+        <v>0.31000000000000005</v>
+      </c>
+      <c r="AA7" s="107">
+        <f>MAX(Tabla2[[#This Row],[Q1]:[Q2]])-MIN(Tabla2[[#This Row],[Q1]:[Q2]])</f>
+        <v>0.20000000000000018</v>
+      </c>
+      <c r="AB7" s="127">
+        <f t="shared" si="2"/>
+        <v>0.31000000000000005</v>
+      </c>
+      <c r="AC7" s="127">
+        <f t="shared" si="3"/>
+        <v>0.10999999999999988</v>
+      </c>
+      <c r="AD7" s="105">
+        <f>AVERAGE(W7:Y7)</f>
+        <v>1.57</v>
+      </c>
+      <c r="AE7" s="105">
+        <f>_xlfn.STDEV.S(W7:Y7)</f>
+        <v>0.15716233645501715</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="56">
         <f>Avg_Match!E29</f>
         <v>1.7</v>
@@ -34926,11 +35620,11 @@
         <v>5</v>
       </c>
       <c r="H8" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.17627106874985649</v>
       </c>
       <c r="I8" s="121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4.3772241374080395E-2</v>
       </c>
       <c r="K8" s="51">
@@ -34941,8 +35635,41 @@
         <f t="shared" si="1"/>
         <v>0.17627106874985649</v>
       </c>
+      <c r="W8" s="126">
+        <v>2.1</v>
+      </c>
+      <c r="X8" s="105">
+        <v>1.89</v>
+      </c>
+      <c r="Y8" s="105">
+        <v>2.4</v>
+      </c>
+      <c r="Z8" s="105">
+        <f>MAX(W8:Y8)-MIN(W8:Y8)</f>
+        <v>0.51</v>
+      </c>
+      <c r="AA8" s="107">
+        <f>MAX(Tabla2[[#This Row],[Q1]:[Q2]])-MIN(Tabla2[[#This Row],[Q1]:[Q2]])</f>
+        <v>0.21000000000000019</v>
+      </c>
+      <c r="AB8" s="127">
+        <f t="shared" si="2"/>
+        <v>0.29999999999999982</v>
+      </c>
+      <c r="AC8" s="127">
+        <f t="shared" si="3"/>
+        <v>0.51</v>
+      </c>
+      <c r="AD8" s="105">
+        <f>AVERAGE(W8:Y8)</f>
+        <v>2.1300000000000003</v>
+      </c>
+      <c r="AE8" s="105">
+        <f>_xlfn.STDEV.S(W8:Y8)</f>
+        <v>0.2563201123595259</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="56">
         <f>Avg_Match!E30</f>
         <v>1.8333330000000001</v>
@@ -34964,11 +35691,11 @@
         <v>6</v>
       </c>
       <c r="H9" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.22343641035541539</v>
       </c>
       <c r="I9" s="121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.0494125397238465E-2</v>
       </c>
       <c r="K9" s="51">
@@ -34979,8 +35706,41 @@
         <f t="shared" si="1"/>
         <v>0.22343641035541539</v>
       </c>
+      <c r="W9" s="126">
+        <v>2.25</v>
+      </c>
+      <c r="X9" s="105">
+        <v>1.8</v>
+      </c>
+      <c r="Y9" s="105">
+        <v>1.5</v>
+      </c>
+      <c r="Z9" s="105">
+        <f>MAX(W9:Y9)-MIN(W9:Y9)</f>
+        <v>0.75</v>
+      </c>
+      <c r="AA9" s="107">
+        <f>MAX(Tabla2[[#This Row],[Q1]:[Q2]])-MIN(Tabla2[[#This Row],[Q1]:[Q2]])</f>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="AB9" s="127">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
+      </c>
+      <c r="AC9" s="127">
+        <f t="shared" si="3"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="AD9" s="105">
+        <f>AVERAGE(W9:Y9)</f>
+        <v>1.8499999999999999</v>
+      </c>
+      <c r="AE9" s="105">
+        <f>_xlfn.STDEV.S(W9:Y9)</f>
+        <v>0.37749172176353757</v>
+      </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="56">
         <f>Avg_Match!E31</f>
         <v>2</v>
@@ -35002,11 +35762,11 @@
         <v>7</v>
       </c>
       <c r="H10" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.27705656503472276</v>
       </c>
       <c r="I10" s="121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.6607569614147216E-2</v>
       </c>
       <c r="K10" s="51">
@@ -35017,8 +35777,41 @@
         <f t="shared" si="1"/>
         <v>0.27705656503472276</v>
       </c>
+      <c r="W10" s="126">
+        <v>1.98</v>
+      </c>
+      <c r="X10" s="105">
+        <v>1.7</v>
+      </c>
+      <c r="Y10" s="105">
+        <v>1.45</v>
+      </c>
+      <c r="Z10" s="105">
+        <f>MAX(W10:Y10)-MIN(W10:Y10)</f>
+        <v>0.53</v>
+      </c>
+      <c r="AA10" s="107">
+        <f>MAX(Tabla2[[#This Row],[Q1]:[Q2]])-MIN(Tabla2[[#This Row],[Q1]:[Q2]])</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AB10" s="127">
+        <f t="shared" si="2"/>
+        <v>0.53</v>
+      </c>
+      <c r="AC10" s="127">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="AD10" s="105">
+        <f>AVERAGE(W10:Y10)</f>
+        <v>1.71</v>
+      </c>
+      <c r="AE10" s="105">
+        <f>_xlfn.STDEV.S(W10:Y10)</f>
+        <v>0.26514147167125796</v>
+      </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="56">
         <f>Avg_Match!E32</f>
         <v>1.7</v>
@@ -35040,11 +35833,11 @@
         <v>8</v>
       </c>
       <c r="H11" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.33630190872075827</v>
       </c>
       <c r="I11" s="121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.167366403107255E-2</v>
       </c>
       <c r="K11" s="51">
@@ -35055,8 +35848,41 @@
         <f t="shared" si="1"/>
         <v>0.33630190872075827</v>
       </c>
+      <c r="W11" s="126">
+        <v>2.1</v>
+      </c>
+      <c r="X11" s="105">
+        <v>4.3</v>
+      </c>
+      <c r="Y11" s="105">
+        <v>2.5</v>
+      </c>
+      <c r="Z11" s="105">
+        <f>MAX(W11:Y11)-MIN(W11:Y11)</f>
+        <v>2.1999999999999997</v>
+      </c>
+      <c r="AA11" s="107">
+        <f>MAX(Tabla2[[#This Row],[Q1]:[Q2]])-MIN(Tabla2[[#This Row],[Q1]:[Q2]])</f>
+        <v>2.1999999999999997</v>
+      </c>
+      <c r="AB11" s="127">
+        <f t="shared" si="2"/>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="AC11" s="127">
+        <f t="shared" si="3"/>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="AD11" s="105">
+        <f>AVERAGE(W11:Y11)</f>
+        <v>2.9666666666666668</v>
+      </c>
+      <c r="AE11" s="105">
+        <f>_xlfn.STDEV.S(W11:Y11)</f>
+        <v>1.1718930554164622</v>
+      </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="56">
         <f>Avg_Match!E33</f>
         <v>1.6666669999999999</v>
@@ -35078,11 +35904,11 @@
         <v>9</v>
       </c>
       <c r="H12" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.39992305283123664</v>
       </c>
       <c r="I12" s="121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.530051075296818E-2</v>
       </c>
       <c r="K12" s="51">
@@ -35093,8 +35919,41 @@
         <f t="shared" si="1"/>
         <v>0.39992305283123664</v>
       </c>
+      <c r="W12" s="130">
+        <v>1.8</v>
+      </c>
+      <c r="X12" s="131">
+        <v>2.15</v>
+      </c>
+      <c r="Y12" s="131">
+        <v>1.5</v>
+      </c>
+      <c r="Z12" s="131">
+        <f>MAX(W12:Y12)-MIN(W12:Y12)</f>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="AA12" s="132">
+        <f>MAX(Tabla2[[#This Row],[Q1]:[Q2]])-MIN(Tabla2[[#This Row],[Q1]:[Q2]])</f>
+        <v>0.34999999999999987</v>
+      </c>
+      <c r="AB12" s="133">
+        <f t="shared" si="2"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="AC12" s="133">
+        <f t="shared" si="3"/>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="AD12" s="131">
+        <f>AVERAGE(W12:Y12)</f>
+        <v>1.8166666666666667</v>
+      </c>
+      <c r="AE12" s="131">
+        <f>_xlfn.STDEV.S(W12:Y12)</f>
+        <v>0.32532035493238642</v>
+      </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="56">
         <f>Avg_Match!E34</f>
         <v>1.9</v>
@@ -35120,7 +35979,7 @@
         <v>0.46632331948293798</v>
       </c>
       <c r="I13" s="121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.7193148565541247E-2</v>
       </c>
       <c r="K13" s="51">
@@ -35132,7 +35991,7 @@
         <v>0.46632331948293798</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="56">
         <f>Avg_Match!E35</f>
         <v>1.8333330000000001</v>
@@ -35154,11 +36013,11 @@
         <v>11</v>
       </c>
       <c r="H14" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.53367668051706207</v>
       </c>
       <c r="I14" s="121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.7193148565541247E-2</v>
       </c>
       <c r="K14" s="51">
@@ -35169,8 +36028,11 @@
         <f t="shared" si="1"/>
         <v>0.53367668051706207</v>
       </c>
+      <c r="W14" s="54">
+        <v>12</v>
+      </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="56">
         <f>Avg_Match!E36</f>
         <v>2</v>
@@ -35192,11 +36054,11 @@
         <v>12</v>
       </c>
       <c r="H15" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.60007694716876336</v>
       </c>
       <c r="I15" s="121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.530051075296818E-2</v>
       </c>
       <c r="K15" s="51">
@@ -35207,8 +36069,20 @@
         <f t="shared" si="1"/>
         <v>0.60007694716876336</v>
       </c>
+      <c r="W15" s="54">
+        <f>W10*$W$14</f>
+        <v>23.759999999999998</v>
+      </c>
+      <c r="X15" s="54">
+        <f t="shared" ref="X15:Y15" si="6">X10*$W$14</f>
+        <v>20.399999999999999</v>
+      </c>
+      <c r="Y15" s="54">
+        <f>Y10*$W$14</f>
+        <v>17.399999999999999</v>
+      </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="56">
         <f>Avg_Match!E37</f>
         <v>2.0333329999999998</v>
@@ -35230,11 +36104,11 @@
         <v>13</v>
       </c>
       <c r="H16" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.66369809127924173</v>
       </c>
       <c r="I16" s="121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.167366403107255E-2</v>
       </c>
       <c r="K16" s="51">
@@ -35268,11 +36142,11 @@
         <v>14</v>
       </c>
       <c r="H17" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.72294343496527724</v>
       </c>
       <c r="I17" s="121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.6607569614147216E-2</v>
       </c>
       <c r="K17" s="51">
@@ -35306,11 +36180,11 @@
         <v>15</v>
       </c>
       <c r="H18" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.77656358964458461</v>
       </c>
       <c r="I18" s="121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.0494125397238465E-2</v>
       </c>
       <c r="K18" s="51">
@@ -35348,7 +36222,7 @@
         <v>0.82372893125014346</v>
       </c>
       <c r="I19" s="121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4.3772241374080395E-2</v>
       </c>
       <c r="K19" s="51">
@@ -35382,11 +36256,11 @@
         <v>17</v>
       </c>
       <c r="H20" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.86405064459017578</v>
       </c>
       <c r="I20" s="121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.687638179856368E-2</v>
       </c>
       <c r="K20" s="51">
@@ -35420,11 +36294,11 @@
         <v>18</v>
       </c>
       <c r="H21" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.89755305309181077</v>
       </c>
       <c r="I21" s="121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.019182784072922E-2</v>
       </c>
       <c r="K21" s="51">
@@ -35458,11 +36332,11 @@
         <v>19</v>
       </c>
       <c r="H22" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.92460721748601438</v>
       </c>
       <c r="I22" s="121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.4022715404011696E-2</v>
       </c>
       <c r="K22" s="51">
@@ -35500,7 +36374,7 @@
         <v>0.94584030963499799</v>
       </c>
       <c r="I23" s="121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.8575750633576825E-2</v>
       </c>
       <c r="K23" s="51">
@@ -35629,7 +36503,7 @@
         <v>5</v>
       </c>
       <c r="C34" s="107">
-        <f t="shared" ref="C34:C65" si="4">B34/D$33</f>
+        <f t="shared" ref="C34:C65" si="7">B34/D$33</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="H34" s="51">
@@ -35645,7 +36519,7 @@
         <v>6</v>
       </c>
       <c r="C35" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.2</v>
       </c>
       <c r="H35" s="51">
@@ -35661,7 +36535,7 @@
         <v>7</v>
       </c>
       <c r="C36" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.23333333333333334</v>
       </c>
       <c r="H36" s="51">
@@ -35677,7 +36551,7 @@
         <v>8</v>
       </c>
       <c r="C37" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.26666666666666666</v>
       </c>
       <c r="H37" s="51">
@@ -35693,14 +36567,14 @@
         <v>9</v>
       </c>
       <c r="C38" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.3</v>
       </c>
       <c r="H38" s="51">
         <v>25</v>
       </c>
       <c r="I38" s="107">
-        <f t="shared" ref="I38:I101" si="5">H38/J$32</f>
+        <f t="shared" ref="I38:I101" si="8">H38/J$32</f>
         <v>0.625</v>
       </c>
     </row>
@@ -35709,14 +36583,14 @@
         <v>10</v>
       </c>
       <c r="C39" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H39" s="51">
         <v>26</v>
       </c>
       <c r="I39" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.65</v>
       </c>
     </row>
@@ -35725,14 +36599,14 @@
         <v>11</v>
       </c>
       <c r="C40" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.36666666666666664</v>
       </c>
       <c r="H40" s="51">
         <v>27</v>
       </c>
       <c r="I40" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.67500000000000004</v>
       </c>
     </row>
@@ -35741,14 +36615,14 @@
         <v>12</v>
       </c>
       <c r="C41" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.4</v>
       </c>
       <c r="H41" s="51">
         <v>28</v>
       </c>
       <c r="I41" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.7</v>
       </c>
     </row>
@@ -35757,14 +36631,14 @@
         <v>13</v>
       </c>
       <c r="C42" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.43333333333333335</v>
       </c>
       <c r="H42" s="51">
         <v>29</v>
       </c>
       <c r="I42" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.72499999999999998</v>
       </c>
     </row>
@@ -35773,14 +36647,14 @@
         <v>14</v>
       </c>
       <c r="C43" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.46666666666666667</v>
       </c>
       <c r="H43" s="51">
         <v>30</v>
       </c>
       <c r="I43" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.75</v>
       </c>
     </row>
@@ -35789,14 +36663,14 @@
         <v>15</v>
       </c>
       <c r="C44" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
       <c r="H44" s="51">
         <v>31</v>
       </c>
       <c r="I44" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.77500000000000002</v>
       </c>
     </row>
@@ -35805,14 +36679,14 @@
         <v>16</v>
       </c>
       <c r="C45" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.53333333333333333</v>
       </c>
       <c r="H45" s="51">
         <v>32</v>
       </c>
       <c r="I45" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.8</v>
       </c>
     </row>
@@ -35821,14 +36695,14 @@
         <v>17</v>
       </c>
       <c r="C46" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.56666666666666665</v>
       </c>
       <c r="H46" s="51">
         <v>33</v>
       </c>
       <c r="I46" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.82499999999999996</v>
       </c>
     </row>
@@ -35837,14 +36711,14 @@
         <v>18</v>
       </c>
       <c r="C47" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.6</v>
       </c>
       <c r="H47" s="51">
         <v>34</v>
       </c>
       <c r="I47" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.85</v>
       </c>
     </row>
@@ -35853,14 +36727,14 @@
         <v>19</v>
       </c>
       <c r="C48" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.6333333333333333</v>
       </c>
       <c r="H48" s="51">
         <v>35</v>
       </c>
       <c r="I48" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.875</v>
       </c>
     </row>
@@ -35869,14 +36743,14 @@
         <v>20</v>
       </c>
       <c r="C49" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="H49" s="51">
         <v>36</v>
       </c>
       <c r="I49" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.9</v>
       </c>
     </row>
@@ -35885,14 +36759,14 @@
         <v>21</v>
       </c>
       <c r="C50" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.7</v>
       </c>
       <c r="H50" s="51">
         <v>37</v>
       </c>
       <c r="I50" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.92500000000000004</v>
       </c>
     </row>
@@ -35901,14 +36775,14 @@
         <v>22</v>
       </c>
       <c r="C51" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.73333333333333328</v>
       </c>
       <c r="H51" s="51">
         <v>38</v>
       </c>
       <c r="I51" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.95</v>
       </c>
     </row>
@@ -35917,14 +36791,14 @@
         <v>23</v>
       </c>
       <c r="C52" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.76666666666666672</v>
       </c>
       <c r="H52" s="51">
         <v>39</v>
       </c>
       <c r="I52" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.97499999999999998</v>
       </c>
     </row>
@@ -35933,14 +36807,14 @@
         <v>24</v>
       </c>
       <c r="C53" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.8</v>
       </c>
       <c r="H53" s="51">
         <v>40</v>
       </c>
       <c r="I53" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -35949,14 +36823,14 @@
         <v>25</v>
       </c>
       <c r="C54" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="H54" s="51">
         <v>41</v>
       </c>
       <c r="I54" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.0249999999999999</v>
       </c>
     </row>
@@ -35965,14 +36839,14 @@
         <v>26</v>
       </c>
       <c r="C55" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.8666666666666667</v>
       </c>
       <c r="H55" s="51">
         <v>42</v>
       </c>
       <c r="I55" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.05</v>
       </c>
     </row>
@@ -35981,14 +36855,14 @@
         <v>27</v>
       </c>
       <c r="C56" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.9</v>
       </c>
       <c r="H56" s="51">
         <v>43</v>
       </c>
       <c r="I56" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.075</v>
       </c>
     </row>
@@ -35997,14 +36871,14 @@
         <v>28</v>
       </c>
       <c r="C57" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.93333333333333335</v>
       </c>
       <c r="H57" s="51">
         <v>44</v>
       </c>
       <c r="I57" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -36013,14 +36887,14 @@
         <v>29</v>
       </c>
       <c r="C58" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.96666666666666667</v>
       </c>
       <c r="H58" s="51">
         <v>45</v>
       </c>
       <c r="I58" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.125</v>
       </c>
     </row>
@@ -36029,14 +36903,14 @@
         <v>30</v>
       </c>
       <c r="C59" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H59" s="51">
         <v>46</v>
       </c>
       <c r="I59" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.1499999999999999</v>
       </c>
     </row>
@@ -36045,14 +36919,14 @@
         <v>31</v>
       </c>
       <c r="C60" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.0333333333333334</v>
       </c>
       <c r="H60" s="51">
         <v>47</v>
       </c>
       <c r="I60" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.175</v>
       </c>
     </row>
@@ -36061,14 +36935,14 @@
         <v>32</v>
       </c>
       <c r="C61" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.0666666666666667</v>
       </c>
       <c r="H61" s="51">
         <v>48</v>
       </c>
       <c r="I61" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.2</v>
       </c>
     </row>
@@ -36077,14 +36951,14 @@
         <v>33</v>
       </c>
       <c r="C62" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="H62" s="51">
         <v>49</v>
       </c>
       <c r="I62" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.2250000000000001</v>
       </c>
     </row>
@@ -36093,14 +36967,14 @@
         <v>34</v>
       </c>
       <c r="C63" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.1333333333333333</v>
       </c>
       <c r="H63" s="51">
         <v>50</v>
       </c>
       <c r="I63" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.25</v>
       </c>
     </row>
@@ -36109,14 +36983,14 @@
         <v>35</v>
       </c>
       <c r="C64" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.1666666666666667</v>
       </c>
       <c r="H64" s="51">
         <v>51</v>
       </c>
       <c r="I64" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.2749999999999999</v>
       </c>
     </row>
@@ -36125,14 +36999,14 @@
         <v>36</v>
       </c>
       <c r="C65" s="107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.2</v>
       </c>
       <c r="H65" s="51">
         <v>52</v>
       </c>
       <c r="I65" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.3</v>
       </c>
     </row>
@@ -36141,14 +37015,14 @@
         <v>37</v>
       </c>
       <c r="C66" s="107">
-        <f t="shared" ref="C66:C97" si="6">B66/D$33</f>
+        <f t="shared" ref="C66:C97" si="9">B66/D$33</f>
         <v>1.2333333333333334</v>
       </c>
       <c r="H66" s="51">
         <v>53</v>
       </c>
       <c r="I66" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.325</v>
       </c>
     </row>
@@ -36157,14 +37031,14 @@
         <v>38</v>
       </c>
       <c r="C67" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.2666666666666666</v>
       </c>
       <c r="H67" s="51">
         <v>54</v>
       </c>
       <c r="I67" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.35</v>
       </c>
     </row>
@@ -36173,14 +37047,14 @@
         <v>39</v>
       </c>
       <c r="C68" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.3</v>
       </c>
       <c r="H68" s="51">
         <v>55</v>
       </c>
       <c r="I68" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.375</v>
       </c>
     </row>
@@ -36189,14 +37063,14 @@
         <v>40</v>
       </c>
       <c r="C69" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="H69" s="51">
         <v>56</v>
       </c>
       <c r="I69" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.4</v>
       </c>
     </row>
@@ -36205,14 +37079,14 @@
         <v>41</v>
       </c>
       <c r="C70" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.3666666666666667</v>
       </c>
       <c r="H70" s="51">
         <v>57</v>
       </c>
       <c r="I70" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.425</v>
       </c>
     </row>
@@ -36221,14 +37095,14 @@
         <v>42</v>
       </c>
       <c r="C71" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.4</v>
       </c>
       <c r="H71" s="51">
         <v>58</v>
       </c>
       <c r="I71" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.45</v>
       </c>
     </row>
@@ -36237,14 +37111,14 @@
         <v>43</v>
       </c>
       <c r="C72" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.4333333333333333</v>
       </c>
       <c r="H72" s="51">
         <v>59</v>
       </c>
       <c r="I72" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.4750000000000001</v>
       </c>
     </row>
@@ -36253,14 +37127,14 @@
         <v>44</v>
       </c>
       <c r="C73" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.4666666666666666</v>
       </c>
       <c r="H73" s="51">
         <v>60</v>
       </c>
       <c r="I73" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.5</v>
       </c>
     </row>
@@ -36269,14 +37143,14 @@
         <v>45</v>
       </c>
       <c r="C74" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.5</v>
       </c>
       <c r="H74" s="51">
         <v>61</v>
       </c>
       <c r="I74" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.5249999999999999</v>
       </c>
       <c r="J74" s="107">
@@ -36288,7 +37162,7 @@
         <v>46</v>
       </c>
       <c r="C75" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.5333333333333334</v>
       </c>
       <c r="D75" s="107">
@@ -36300,7 +37174,7 @@
         <v>62</v>
       </c>
       <c r="I75" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.55</v>
       </c>
     </row>
@@ -36309,7 +37183,7 @@
         <v>47</v>
       </c>
       <c r="C76" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.5666666666666667</v>
       </c>
       <c r="D76" s="104"/>
@@ -36319,7 +37193,7 @@
         <v>63</v>
       </c>
       <c r="I76" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.575</v>
       </c>
     </row>
@@ -36328,7 +37202,7 @@
         <v>48</v>
       </c>
       <c r="C77" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.6</v>
       </c>
       <c r="D77" s="104"/>
@@ -36338,7 +37212,7 @@
         <v>64</v>
       </c>
       <c r="I77" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.6</v>
       </c>
     </row>
@@ -36347,7 +37221,7 @@
         <v>49</v>
       </c>
       <c r="C78" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.6333333333333333</v>
       </c>
       <c r="D78" s="107">
@@ -36361,7 +37235,7 @@
         <v>65</v>
       </c>
       <c r="I78" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.625</v>
       </c>
     </row>
@@ -36370,14 +37244,14 @@
         <v>50</v>
       </c>
       <c r="C79" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="H79" s="51">
         <v>66</v>
       </c>
       <c r="I79" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.65</v>
       </c>
     </row>
@@ -36386,7 +37260,7 @@
         <v>51</v>
       </c>
       <c r="C80" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.7</v>
       </c>
       <c r="D80" s="107">
@@ -36400,7 +37274,7 @@
         <v>67</v>
       </c>
       <c r="I80" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.675</v>
       </c>
       <c r="J80" s="107">
@@ -36412,14 +37286,14 @@
         <v>52</v>
       </c>
       <c r="C81" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.7333333333333334</v>
       </c>
       <c r="H81" s="51">
         <v>68</v>
       </c>
       <c r="I81" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.7</v>
       </c>
     </row>
@@ -36428,14 +37302,14 @@
         <v>53</v>
       </c>
       <c r="C82" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.7666666666666666</v>
       </c>
       <c r="H82" s="51">
         <v>69</v>
       </c>
       <c r="I82" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.7250000000000001</v>
       </c>
       <c r="J82" s="107">
@@ -36448,14 +37322,14 @@
         <v>54</v>
       </c>
       <c r="C83" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.8</v>
       </c>
       <c r="H83" s="51">
         <v>70</v>
       </c>
       <c r="I83" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.75</v>
       </c>
       <c r="J83" s="107">
@@ -36467,7 +37341,7 @@
         <v>55</v>
       </c>
       <c r="C84" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.8333333333333333</v>
       </c>
       <c r="D84" s="107">
@@ -36483,7 +37357,7 @@
         <v>71</v>
       </c>
       <c r="I84" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.7749999999999999</v>
       </c>
     </row>
@@ -36492,7 +37366,7 @@
         <v>56</v>
       </c>
       <c r="C85" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.8666666666666667</v>
       </c>
       <c r="D85" s="107">
@@ -36504,7 +37378,7 @@
         <v>72</v>
       </c>
       <c r="I85" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.8</v>
       </c>
       <c r="J85" s="107">
@@ -36519,7 +37393,7 @@
         <v>57</v>
       </c>
       <c r="C86" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.9</v>
       </c>
       <c r="D86" s="107">
@@ -36531,7 +37405,7 @@
         <v>73</v>
       </c>
       <c r="I86" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.825</v>
       </c>
     </row>
@@ -36540,7 +37414,7 @@
         <v>58</v>
       </c>
       <c r="C87" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.9333333333333333</v>
       </c>
       <c r="D87" s="104"/>
@@ -36549,7 +37423,7 @@
         <v>74</v>
       </c>
       <c r="I87" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.85</v>
       </c>
       <c r="J87" s="107">
@@ -36561,7 +37435,7 @@
         <v>59</v>
       </c>
       <c r="C88" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.9666666666666666</v>
       </c>
       <c r="D88" s="104"/>
@@ -36570,7 +37444,7 @@
         <v>75</v>
       </c>
       <c r="I88" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.875</v>
       </c>
     </row>
@@ -36579,7 +37453,7 @@
         <v>60</v>
       </c>
       <c r="C89" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="D89" s="107">
@@ -36593,7 +37467,7 @@
         <v>76</v>
       </c>
       <c r="I89" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.9</v>
       </c>
       <c r="J89" s="107">
@@ -36605,7 +37479,7 @@
         <v>61</v>
       </c>
       <c r="C90" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2.0333333333333332</v>
       </c>
       <c r="D90" s="107">
@@ -36616,7 +37490,7 @@
         <v>77</v>
       </c>
       <c r="I90" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.925</v>
       </c>
       <c r="J90" s="107">
@@ -36628,7 +37502,7 @@
         <v>62</v>
       </c>
       <c r="C91" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2.0666666666666669</v>
       </c>
       <c r="D91" s="107">
@@ -36639,7 +37513,7 @@
         <v>78</v>
       </c>
       <c r="I91" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.95</v>
       </c>
     </row>
@@ -36648,7 +37522,7 @@
         <v>63</v>
       </c>
       <c r="C92" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2.1</v>
       </c>
       <c r="D92" s="107">
@@ -36658,7 +37532,7 @@
         <v>79</v>
       </c>
       <c r="I92" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.9750000000000001</v>
       </c>
       <c r="J92" s="107">
@@ -36670,14 +37544,14 @@
         <v>64</v>
       </c>
       <c r="C93" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2.1333333333333333</v>
       </c>
       <c r="H93" s="51">
         <v>80</v>
       </c>
       <c r="I93" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="J93" s="107">
@@ -36692,7 +37566,7 @@
         <v>65</v>
       </c>
       <c r="C94" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2.1666666666666665</v>
       </c>
       <c r="D94" s="107">
@@ -36702,7 +37576,7 @@
         <v>81</v>
       </c>
       <c r="I94" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.0249999999999999</v>
       </c>
     </row>
@@ -36711,7 +37585,7 @@
         <v>66</v>
       </c>
       <c r="C95" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2.2000000000000002</v>
       </c>
       <c r="D95" s="107">
@@ -36724,7 +37598,7 @@
         <v>82</v>
       </c>
       <c r="I95" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.0499999999999998</v>
       </c>
       <c r="J95" s="107">
@@ -36736,14 +37610,14 @@
         <v>67</v>
       </c>
       <c r="C96" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2.2333333333333334</v>
       </c>
       <c r="H96" s="51">
         <v>83</v>
       </c>
       <c r="I96" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.0750000000000002</v>
       </c>
       <c r="J96" s="107">
@@ -36755,14 +37629,14 @@
         <v>68</v>
       </c>
       <c r="C97" s="107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2.2666666666666666</v>
       </c>
       <c r="H97" s="51">
         <v>84</v>
       </c>
       <c r="I97" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.1</v>
       </c>
       <c r="J97" s="107">
@@ -36774,7 +37648,7 @@
         <v>69</v>
       </c>
       <c r="C98" s="107">
-        <f t="shared" ref="C98:C129" si="7">B98/D$33</f>
+        <f t="shared" ref="C98:C129" si="10">B98/D$33</f>
         <v>2.2999999999999998</v>
       </c>
       <c r="D98" s="107">
@@ -36785,7 +37659,7 @@
         <v>85</v>
       </c>
       <c r="I98" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.125</v>
       </c>
       <c r="J98" s="107">
@@ -36797,7 +37671,7 @@
         <v>70</v>
       </c>
       <c r="C99" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2.3333333333333335</v>
       </c>
       <c r="E99" s="104"/>
@@ -36805,7 +37679,7 @@
         <v>86</v>
       </c>
       <c r="I99" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.15</v>
       </c>
     </row>
@@ -36814,7 +37688,7 @@
         <v>71</v>
       </c>
       <c r="C100" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2.3666666666666667</v>
       </c>
       <c r="D100" s="104"/>
@@ -36824,7 +37698,7 @@
         <v>87</v>
       </c>
       <c r="I100" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.1749999999999998</v>
       </c>
       <c r="J100" s="107">
@@ -36836,7 +37710,7 @@
         <v>72</v>
       </c>
       <c r="C101" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2.4</v>
       </c>
       <c r="D101" s="104"/>
@@ -36846,7 +37720,7 @@
         <v>88</v>
       </c>
       <c r="I101" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.2000000000000002</v>
       </c>
       <c r="J101" s="107">
@@ -36858,7 +37732,7 @@
         <v>73</v>
       </c>
       <c r="C102" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2.4333333333333331</v>
       </c>
       <c r="D102" s="104"/>
@@ -36868,7 +37742,7 @@
         <v>89</v>
       </c>
       <c r="I102" s="107">
-        <f t="shared" ref="I102:I132" si="8">H102/J$32</f>
+        <f t="shared" ref="I102:I132" si="11">H102/J$32</f>
         <v>2.2250000000000001</v>
       </c>
     </row>
@@ -36877,7 +37751,7 @@
         <v>74</v>
       </c>
       <c r="C103" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2.4666666666666668</v>
       </c>
       <c r="D103" s="107">
@@ -36889,7 +37763,7 @@
         <v>90</v>
       </c>
       <c r="I103" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.25</v>
       </c>
     </row>
@@ -36898,7 +37772,7 @@
         <v>75</v>
       </c>
       <c r="C104" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2.5</v>
       </c>
       <c r="D104" s="104"/>
@@ -36908,7 +37782,7 @@
         <v>91</v>
       </c>
       <c r="I104" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.2749999999999999</v>
       </c>
       <c r="J104" s="107">
@@ -36920,7 +37794,7 @@
         <v>76</v>
       </c>
       <c r="C105" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2.5333333333333332</v>
       </c>
       <c r="D105" s="104"/>
@@ -36930,7 +37804,7 @@
         <v>92</v>
       </c>
       <c r="I105" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.2999999999999998</v>
       </c>
       <c r="J105" s="107">
@@ -36942,7 +37816,7 @@
         <v>77</v>
       </c>
       <c r="C106" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2.5666666666666669</v>
       </c>
       <c r="D106" s="104"/>
@@ -36952,7 +37826,7 @@
         <v>93</v>
       </c>
       <c r="I106" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.3250000000000002</v>
       </c>
     </row>
@@ -36961,7 +37835,7 @@
         <v>78</v>
       </c>
       <c r="C107" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2.6</v>
       </c>
       <c r="D107" s="104"/>
@@ -36971,7 +37845,7 @@
         <v>94</v>
       </c>
       <c r="I107" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.35</v>
       </c>
     </row>
@@ -36980,7 +37854,7 @@
         <v>79</v>
       </c>
       <c r="C108" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2.6333333333333333</v>
       </c>
       <c r="D108" s="104"/>
@@ -36990,7 +37864,7 @@
         <v>95</v>
       </c>
       <c r="I108" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.375</v>
       </c>
     </row>
@@ -36999,7 +37873,7 @@
         <v>80</v>
       </c>
       <c r="C109" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2.6666666666666665</v>
       </c>
       <c r="D109" s="104"/>
@@ -37009,7 +37883,7 @@
         <v>96</v>
       </c>
       <c r="I109" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.4</v>
       </c>
     </row>
@@ -37018,14 +37892,14 @@
         <v>81</v>
       </c>
       <c r="C110" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2.7</v>
       </c>
       <c r="H110" s="51">
         <v>97</v>
       </c>
       <c r="I110" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.4249999999999998</v>
       </c>
     </row>
@@ -37034,14 +37908,14 @@
         <v>82</v>
       </c>
       <c r="C111" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2.7333333333333334</v>
       </c>
       <c r="H111" s="51">
         <v>98</v>
       </c>
       <c r="I111" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.4500000000000002</v>
       </c>
     </row>
@@ -37050,14 +37924,14 @@
         <v>83</v>
       </c>
       <c r="C112" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2.7666666666666666</v>
       </c>
       <c r="H112" s="51">
         <v>99</v>
       </c>
       <c r="I112" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.4750000000000001</v>
       </c>
     </row>
@@ -37066,14 +37940,14 @@
         <v>84</v>
       </c>
       <c r="C113" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2.8</v>
       </c>
       <c r="H113" s="51">
         <v>100</v>
       </c>
       <c r="I113" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.5</v>
       </c>
     </row>
@@ -37082,14 +37956,14 @@
         <v>85</v>
       </c>
       <c r="C114" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2.8333333333333335</v>
       </c>
       <c r="H114" s="51">
         <v>101</v>
       </c>
       <c r="I114" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.5249999999999999</v>
       </c>
     </row>
@@ -37098,14 +37972,14 @@
         <v>86</v>
       </c>
       <c r="C115" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2.8666666666666667</v>
       </c>
       <c r="H115" s="51">
         <v>102</v>
       </c>
       <c r="I115" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.5499999999999998</v>
       </c>
     </row>
@@ -37114,14 +37988,14 @@
         <v>87</v>
       </c>
       <c r="C116" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2.9</v>
       </c>
       <c r="H116" s="51">
         <v>103</v>
       </c>
       <c r="I116" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.5750000000000002</v>
       </c>
     </row>
@@ -37130,14 +38004,14 @@
         <v>88</v>
       </c>
       <c r="C117" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2.9333333333333331</v>
       </c>
       <c r="H117" s="51">
         <v>104</v>
       </c>
       <c r="I117" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.6</v>
       </c>
     </row>
@@ -37146,14 +38020,14 @@
         <v>89</v>
       </c>
       <c r="C118" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2.9666666666666668</v>
       </c>
       <c r="H118" s="51">
         <v>105</v>
       </c>
       <c r="I118" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.625</v>
       </c>
     </row>
@@ -37162,14 +38036,14 @@
         <v>90</v>
       </c>
       <c r="C119" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="H119" s="51">
         <v>106</v>
       </c>
       <c r="I119" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.65</v>
       </c>
     </row>
@@ -37178,14 +38052,14 @@
         <v>91</v>
       </c>
       <c r="C120" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>3.0333333333333332</v>
       </c>
       <c r="H120" s="51">
         <v>107</v>
       </c>
       <c r="I120" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.6749999999999998</v>
       </c>
     </row>
@@ -37194,14 +38068,14 @@
         <v>92</v>
       </c>
       <c r="C121" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>3.0666666666666669</v>
       </c>
       <c r="H121" s="51">
         <v>108</v>
       </c>
       <c r="I121" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.7</v>
       </c>
     </row>
@@ -37210,14 +38084,14 @@
         <v>93</v>
       </c>
       <c r="C122" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>3.1</v>
       </c>
       <c r="H122" s="51">
         <v>109</v>
       </c>
       <c r="I122" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.7250000000000001</v>
       </c>
     </row>
@@ -37226,14 +38100,14 @@
         <v>94</v>
       </c>
       <c r="C123" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>3.1333333333333333</v>
       </c>
       <c r="H123" s="51">
         <v>110</v>
       </c>
       <c r="I123" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.75</v>
       </c>
     </row>
@@ -37242,14 +38116,14 @@
         <v>95</v>
       </c>
       <c r="C124" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>3.1666666666666665</v>
       </c>
       <c r="H124" s="51">
         <v>111</v>
       </c>
       <c r="I124" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.7749999999999999</v>
       </c>
     </row>
@@ -37258,14 +38132,14 @@
         <v>96</v>
       </c>
       <c r="C125" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>3.2</v>
       </c>
       <c r="H125" s="51">
         <v>112</v>
       </c>
       <c r="I125" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.8</v>
       </c>
     </row>
@@ -37274,14 +38148,14 @@
         <v>97</v>
       </c>
       <c r="C126" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>3.2333333333333334</v>
       </c>
       <c r="H126" s="51">
         <v>113</v>
       </c>
       <c r="I126" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.8250000000000002</v>
       </c>
     </row>
@@ -37290,14 +38164,14 @@
         <v>98</v>
       </c>
       <c r="C127" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>3.2666666666666666</v>
       </c>
       <c r="H127" s="51">
         <v>114</v>
       </c>
       <c r="I127" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.85</v>
       </c>
     </row>
@@ -37306,14 +38180,14 @@
         <v>99</v>
       </c>
       <c r="C128" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>3.3</v>
       </c>
       <c r="H128" s="51">
         <v>115</v>
       </c>
       <c r="I128" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.875</v>
       </c>
     </row>
@@ -37322,14 +38196,14 @@
         <v>100</v>
       </c>
       <c r="C129" s="107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="H129" s="51">
         <v>116</v>
       </c>
       <c r="I129" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.9</v>
       </c>
     </row>
@@ -37338,7 +38212,7 @@
         <v>117</v>
       </c>
       <c r="I130" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.9249999999999998</v>
       </c>
     </row>
@@ -37347,7 +38221,7 @@
         <v>118</v>
       </c>
       <c r="I131" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.95</v>
       </c>
     </row>
@@ -37356,7 +38230,7 @@
         <v>119</v>
       </c>
       <c r="I132" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.9750000000000001</v>
       </c>
     </row>
@@ -37422,9 +38296,68 @@
     <sortCondition ref="D4:D23"/>
   </sortState>
   <phoneticPr fontId="8" type="noConversion"/>
+  <conditionalFormatting sqref="W4:Z12 AD4:AE12 AA4:AC4">
+    <cfRule type="dataBar" priority="22">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{811ED4DF-090A-491B-8517-E26BCD08A1AE}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA4:AC12">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{3DEFEFA2-256B-453E-B5A1-41D4ABA999D1}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{811ED4DF-090A-491B-8517-E26BCD08A1AE}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>W4:Z12 AD4:AE12 AA4:AC4</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{3DEFEFA2-256B-453E-B5A1-41D4ABA999D1}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>AA4:AC12</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -37432,7 +38365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D0F9BD-4379-4405-B793-B04BABC99C18}">
   <dimension ref="C1:N30"/>
   <sheetViews>
-    <sheetView topLeftCell="B20" workbookViewId="0">
+    <sheetView topLeftCell="B5" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>